<commit_message>
update image and roeiro
</commit_message>
<xml_diff>
--- a/Demo Excel/file/Dados.xlsx
+++ b/Demo Excel/file/Dados.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D23FAA-55B2-41E0-A01C-3A5D90EBF10B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C01C87E-8CBE-4184-BA58-B7AF759D60F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Customer</t>
   </si>
@@ -71,6 +72,9 @@
   </si>
   <si>
     <t>Q3</t>
+  </si>
+  <si>
+    <t>Budget</t>
   </si>
 </sst>
 </file>
@@ -135,6 +139,17 @@
     <tableColumn id="4" xr3:uid="{0B1F388D-253A-44D0-9BA0-D05866B9CA92}" name="Forecast"/>
     <tableColumn id="5" xr3:uid="{DCEDFD76-6818-427A-B00C-B0CFAA41A8AF}" name="Quarter"/>
     <tableColumn id="6" xr3:uid="{0A9BBD85-049A-4477-888E-684533C63F46}" name="Fiscal Year"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC0444EF-A9E4-4ECB-A76F-CEFAC152E53F}" name="Budget" displayName="Budget" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4" xr:uid="{9E359ABF-2346-4547-9981-B23323DC2985}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{059FEFFF-3B3D-4E33-8D59-4C32403B4A9E}" name="Owner"/>
+    <tableColumn id="2" xr3:uid="{31DEC075-6A0C-4B44-81C3-9CAB0FE5BFE9}" name="Budget"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -405,7 +420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -501,4 +516,52 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F43908C-57EB-4A64-BDCB-9F4AEBE6CB19}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>3000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>